<commit_message>
added MNW functionality - minor changes
</commit_message>
<xml_diff>
--- a/testing/test7_semiconf_nogp/results/MNW vs WEL output.xlsx
+++ b/testing/test7_semiconf_nogp/results/MNW vs WEL output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sutra2_tool\sutra2\testing\test7_semiconf_nogp\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6551E160-611F-4072-AEFC-9A7354B08926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DBC7C7-FF99-42C9-868A-34B40DBC9EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{79CFC340-DC7D-47F8-B4AE-3DE3126AD9F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79CFC340-DC7D-47F8-B4AE-3DE3126AD9F9}"/>
   </bookViews>
   <sheets>
     <sheet name="MNW vs WEL package pathlines" sheetId="1" r:id="rId1"/>
@@ -3111,13 +3111,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>125729</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>53339</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>555487</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>93344</xdr:rowOff>
+      <xdr:rowOff>116204</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3140,8 +3140,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13584554" y="2225039"/>
-          <a:ext cx="2879588" cy="2204085"/>
+          <a:off x="16455389" y="2270759"/>
+          <a:ext cx="2868158" cy="2234565"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3321,14 +3321,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>605790</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>426495</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>226098</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>46803</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>15793</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3352,8 +3352,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20770215" y="1114425"/>
-          <a:ext cx="9373908" cy="3968668"/>
+          <a:off x="23474754" y="745752"/>
+          <a:ext cx="9373908" cy="3931688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3744,8 +3744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3450C9-E7C4-4985-8C4F-0E873A9AE869}">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="P16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>